<commit_message>
05-111. Auth Service Setup
</commit_message>
<xml_diff>
--- a/05-105. Big Ticket Items.xlsx
+++ b/05-105. Big Ticket Items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\React\Microservices-with-NodeJS-and-React\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FB3DA8-6A7F-4945-84EC-A208EAB97A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9405A85F-4AC1-482F-B19D-CC6E5B265802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{BF1C9B14-C581-4D08-AFF6-9998005E9F8D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{BF1C9B14-C581-4D08-AFF6-9998005E9F8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Architecutre" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Resources" sheetId="3" r:id="rId3"/>
     <sheet name="Services" sheetId="4" r:id="rId4"/>
     <sheet name="Events" sheetId="5" r:id="rId5"/>
+    <sheet name="Auth Service" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="88">
   <si>
     <t>Items</t>
   </si>
@@ -437,6 +438,52 @@
   <si>
     <t>Events/
 Resources</t>
+  </si>
+  <si>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>/api/users/signup</t>
+  </si>
+  <si>
+    <t>/api/users/signin</t>
+  </si>
+  <si>
+    <t>/api/users/signout</t>
+  </si>
+  <si>
+    <t>/api/users/currentuser</t>
+  </si>
+  <si>
+    <t>Sign up for a new account</t>
+  </si>
+  <si>
+    <t>Sign in to an existing account</t>
+  </si>
+  <si>
+    <t>Sign out</t>
+  </si>
+  <si>
+    <t>Return user info about the user</t>
+  </si>
+  <si>
+    <t>{ email: string,
+   password: string }</t>
   </si>
 </sst>
 </file>
@@ -1242,7 +1289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5E07E6-5F63-4F24-B073-12B820F4C830}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1325,4 +1372,91 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFB6CF0-28E6-45F2-AE02-CA1C6A11E072}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="28" style="9" customWidth="1"/>
+    <col min="4" max="4" width="37" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>